<commit_message>
Added logo features and refactor
</commit_message>
<xml_diff>
--- a/test_modified.xlsx
+++ b/test_modified.xlsx
@@ -471,7 +471,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>C:\Users\Ismail\Desktop\Automation\QR Code Images\1.png</t>
+          <t>E:\Event-Etrance-QR-Code\QR Code Images\1.png</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>C:\Users\Ismail\Desktop\Automation\QR Code Images\2.png</t>
+          <t>E:\Event-Etrance-QR-Code\QR Code Images\2.png</t>
         </is>
       </c>
     </row>
@@ -511,7 +511,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>C:\Users\Ismail\Desktop\Automation\QR Code Images\3.png</t>
+          <t>E:\Event-Etrance-QR-Code\QR Code Images\3.png</t>
         </is>
       </c>
     </row>

</xml_diff>